<commit_message>
Some bom fix. Update all output files.
</commit_message>
<xml_diff>
--- a/Assembly/shield_display_4.3/bom-shield_display_4.3.xlsx
+++ b/Assembly/shield_display_4.3/bom-shield_display_4.3.xlsx
@@ -9,7 +9,7 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
@@ -19,7 +19,7 @@
     <t>Bill of Materials</t>
   </si>
   <si>
-    <t>Date: Tuesday, 09 February 2016 10:58:16</t>
+    <t>Date: Friday, 15 April 2016 17:07:16</t>
   </si>
   <si>
     <t>Project: EVA01 Shield Display 4.3''</t>
@@ -28,7 +28,7 @@
     <t>Hardware_version: 1</t>
   </si>
   <si>
-    <t>PCB_version: A</t>
+    <t>PCB_version: B</t>
   </si>
   <si>
     <t>BOM files:</t>
@@ -91,67 +91,67 @@
     <t>40-pin, 0.5mm, SMT, ZIF, Horizontal, Top Contact (WE 68714014022; Molex: 54104-4031)</t>
   </si>
   <si>
-    <t>J2, J3</t>
+    <t>J1, J2, J3</t>
   </si>
   <si>
     <t>SOCKET_2x26_2.54MM_SMD</t>
   </si>
   <si>
-    <t>Pin header 26x2</t>
-  </si>
-  <si>
-    <t>J1</t>
-  </si>
-  <si>
-    <t>Socket Header, 26 pin, 13x2, 2.54mm, H=8.5mm</t>
+    <t>Socket Header, 52 pin, 26x2, 2.54mm, H=8.5mm</t>
+  </si>
+  <si>
+    <t>R1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NP  </t>
+  </si>
+  <si>
+    <t>0603_[1608]</t>
+  </si>
+  <si>
+    <t>Resistor 0.125W</t>
+  </si>
+  <si>
+    <t>R7, R9, R11, R13, R15, R16, R17</t>
+  </si>
+  <si>
+    <t>Resistor</t>
+  </si>
+  <si>
+    <t>R6, R8, R10, R12, R14, R18, R19</t>
+  </si>
+  <si>
+    <t>0R</t>
+  </si>
+  <si>
+    <t>R2</t>
+  </si>
+  <si>
+    <t>10R 1%</t>
+  </si>
+  <si>
+    <t>R20</t>
+  </si>
+  <si>
+    <t>1k</t>
+  </si>
+  <si>
+    <t>R5</t>
+  </si>
+  <si>
+    <t>220k 1%</t>
   </si>
   <si>
     <t>R3</t>
   </si>
   <si>
-    <t>390K 1%</t>
-  </si>
-  <si>
-    <t>0603_[1608]</t>
-  </si>
-  <si>
-    <t>Resistor</t>
+    <t>390k 1%</t>
   </si>
   <si>
     <t>R4</t>
   </si>
   <si>
-    <t>820K 1%</t>
-  </si>
-  <si>
-    <t>R1</t>
-  </si>
-  <si>
-    <t>NP</t>
-  </si>
-  <si>
-    <t>Resistor 0.125W</t>
-  </si>
-  <si>
-    <t>R7, R9, R11, R13</t>
-  </si>
-  <si>
-    <t>R2</t>
-  </si>
-  <si>
-    <t>10R 1%</t>
-  </si>
-  <si>
-    <t>R5</t>
-  </si>
-  <si>
-    <t>220K 1%</t>
-  </si>
-  <si>
-    <t>R6, R8, R10, R12</t>
-  </si>
-  <si>
-    <t>0R</t>
+    <t>820k 1%</t>
   </si>
   <si>
     <t>C1, C3, C6, C8</t>
@@ -163,6 +163,12 @@
     <t>Ceramic X7R 50V</t>
   </si>
   <si>
+    <t>C7</t>
+  </si>
+  <si>
+    <t>Ceramic X5R 6.3V, 10V</t>
+  </si>
+  <si>
     <t>C4</t>
   </si>
   <si>
@@ -172,12 +178,6 @@
     <t>Ceramic X7R, X5R 16V</t>
   </si>
   <si>
-    <t>C7</t>
-  </si>
-  <si>
-    <t>Ceramic X5R 6.3V, 10V</t>
-  </si>
-  <si>
     <t>C5</t>
   </si>
   <si>
@@ -193,7 +193,7 @@
     <t>L1</t>
   </si>
   <si>
-    <t>22uH - WE 744062220</t>
+    <t>22uH WE 744062220</t>
   </si>
   <si>
     <t>WE-TPC-6823-X</t>
@@ -202,6 +202,18 @@
     <t>Power Inductor</t>
   </si>
   <si>
+    <t>U1</t>
+  </si>
+  <si>
+    <t>24C128</t>
+  </si>
+  <si>
+    <t>SOIC8</t>
+  </si>
+  <si>
+    <t>EEPROM</t>
+  </si>
+  <si>
     <t>U2</t>
   </si>
   <si>
@@ -212,18 +224,6 @@
   </si>
   <si>
     <t>White LED Driver with Integrated Schottky</t>
-  </si>
-  <si>
-    <t>U1</t>
-  </si>
-  <si>
-    <t>24C128</t>
-  </si>
-  <si>
-    <t>SOIC8</t>
-  </si>
-  <si>
-    <t>EEPROM</t>
   </si>
 </sst>
 </file>
@@ -324,7 +324,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -333,9 +333,6 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -344,6 +341,12 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -641,117 +644,121 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F46"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="G15" sqref="G15"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="3" max="46" width="12.7109375" customWidth="1"/>
-    <col min="4" max="46" width="36.7109375" customWidth="1"/>
-    <col min="5" max="46" width="30.7109375" customWidth="1"/>
-    <col min="6" max="46" width="36.7109375" customWidth="1"/>
+    <col min="3" max="3" width="29.5703125" customWidth="1"/>
+    <col min="4" max="4" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="26.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="79.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="11" width="15.7109375" customWidth="1"/>
+    <col min="12" max="46" width="246.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+      <c r="F1" s="7"/>
     </row>
     <row r="2" spans="1:6">
-      <c r="A2" s="1"/>
-      <c r="B2" s="1"/>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
+      <c r="A2" s="7"/>
+      <c r="B2" s="7"/>
+      <c r="C2" s="7"/>
+      <c r="D2" s="7"/>
+      <c r="E2" s="7"/>
+      <c r="F2" s="7"/>
     </row>
     <row r="3" spans="1:6">
-      <c r="A3" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" s="1"/>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
+      <c r="A3" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="7"/>
+      <c r="C3" s="7"/>
+      <c r="D3" s="7"/>
+      <c r="E3" s="7"/>
+      <c r="F3" s="7"/>
     </row>
     <row r="4" spans="1:6">
-      <c r="A4" s="1"/>
-      <c r="B4" s="1"/>
-      <c r="C4" s="1"/>
-      <c r="D4" s="1"/>
-      <c r="E4" s="1"/>
-      <c r="F4" s="1"/>
+      <c r="A4" s="7"/>
+      <c r="B4" s="7"/>
+      <c r="C4" s="7"/>
+      <c r="D4" s="7"/>
+      <c r="E4" s="7"/>
+      <c r="F4" s="7"/>
     </row>
     <row r="5" spans="1:6">
-      <c r="A5" s="1"/>
-      <c r="B5" s="1"/>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
-      <c r="E5" s="1"/>
-      <c r="F5" s="1"/>
+      <c r="A5" s="7"/>
+      <c r="B5" s="7"/>
+      <c r="C5" s="7"/>
+      <c r="D5" s="7"/>
+      <c r="E5" s="7"/>
+      <c r="F5" s="7"/>
     </row>
     <row r="6" spans="1:6">
-      <c r="A6" s="1" t="s">
+      <c r="A6" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="B6" s="1"/>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
-      <c r="E6" s="1"/>
-      <c r="F6" s="1"/>
+      <c r="B6" s="7"/>
+      <c r="C6" s="7"/>
+      <c r="D6" s="7"/>
+      <c r="E6" s="7"/>
+      <c r="F6" s="7"/>
     </row>
     <row r="7" spans="1:6">
-      <c r="A7" s="1" t="s">
+      <c r="A7" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="B7" s="1"/>
-      <c r="C7" s="1"/>
-      <c r="D7" s="1"/>
-      <c r="E7" s="1"/>
-      <c r="F7" s="1"/>
+      <c r="B7" s="7"/>
+      <c r="C7" s="7"/>
+      <c r="D7" s="7"/>
+      <c r="E7" s="7"/>
+      <c r="F7" s="7"/>
     </row>
     <row r="8" spans="1:6">
-      <c r="A8" s="1" t="s">
+      <c r="A8" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="B8" s="1"/>
-      <c r="C8" s="1"/>
-      <c r="D8" s="1"/>
-      <c r="E8" s="1"/>
-      <c r="F8" s="1"/>
+      <c r="B8" s="7"/>
+      <c r="C8" s="7"/>
+      <c r="D8" s="7"/>
+      <c r="E8" s="7"/>
+      <c r="F8" s="7"/>
     </row>
     <row r="9" spans="1:6">
-      <c r="A9" s="1"/>
-      <c r="B9" s="1"/>
-      <c r="C9" s="1"/>
-      <c r="D9" s="1"/>
-      <c r="E9" s="1"/>
-      <c r="F9" s="1"/>
+      <c r="A9" s="7"/>
+      <c r="B9" s="7"/>
+      <c r="C9" s="7"/>
+      <c r="D9" s="7"/>
+      <c r="E9" s="7"/>
+      <c r="F9" s="7"/>
     </row>
     <row r="10" spans="1:6">
-      <c r="A10" s="1" t="s">
+      <c r="A10" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="B10" s="1"/>
-      <c r="C10" s="1"/>
-      <c r="D10" s="1"/>
-      <c r="E10" s="1"/>
-      <c r="F10" s="1"/>
+      <c r="B10" s="7"/>
+      <c r="C10" s="7"/>
+      <c r="D10" s="7"/>
+      <c r="E10" s="7"/>
+      <c r="F10" s="7"/>
     </row>
     <row r="11" spans="1:6">
-      <c r="A11" s="1" t="s">
+      <c r="A11" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="B11" s="1"/>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
-      <c r="E11" s="1"/>
-      <c r="F11" s="1"/>
+      <c r="B11" s="7"/>
+      <c r="C11" s="7"/>
+      <c r="D11" s="7"/>
+      <c r="E11" s="7"/>
+      <c r="F11" s="7"/>
     </row>
     <row r="13" spans="1:6">
       <c r="A13" s="2" t="s">
@@ -789,7 +796,7 @@
     </row>
     <row r="18" spans="1:6">
       <c r="A18" s="1">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>12</v>
@@ -805,13 +812,13 @@
     </row>
     <row r="20" spans="1:6">
       <c r="A20" s="1">
-        <v>27</v>
+        <v>34</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="22" spans="1:6">
+    <row r="22" spans="1:6" ht="15.75">
       <c r="A22" s="3" t="s">
         <v>15</v>
       </c>
@@ -832,413 +839,413 @@
       </c>
     </row>
     <row r="25" spans="1:6">
-      <c r="A25" s="4" t="s">
+      <c r="A25" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="B25" s="4"/>
-      <c r="C25" s="4"/>
-      <c r="D25" s="4"/>
-      <c r="E25" s="4"/>
-      <c r="F25" s="4"/>
+      <c r="B25" s="8"/>
+      <c r="C25" s="8"/>
+      <c r="D25" s="8"/>
+      <c r="E25" s="8"/>
+      <c r="F25" s="8"/>
     </row>
     <row r="26" spans="1:6">
-      <c r="A26" s="5">
-        <v>1</v>
-      </c>
-      <c r="B26" s="6">
-        <v>1</v>
-      </c>
-      <c r="C26" s="6" t="s">
+      <c r="A26" s="4">
+        <v>1</v>
+      </c>
+      <c r="B26" s="5">
+        <v>1</v>
+      </c>
+      <c r="C26" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="D26" s="6" t="s">
+      <c r="D26" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="E26" s="6" t="s">
+      <c r="E26" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="F26" s="6" t="s">
+      <c r="F26" s="5" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="27" spans="1:6">
-      <c r="A27" s="5">
-        <v>2</v>
-      </c>
-      <c r="B27" s="6">
-        <v>2</v>
-      </c>
-      <c r="C27" s="6" t="s">
+      <c r="A27" s="4">
+        <v>3</v>
+      </c>
+      <c r="B27" s="5">
+        <v>3</v>
+      </c>
+      <c r="C27" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="D27" s="6" t="s">
+      <c r="D27" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="E27" s="6" t="s">
+      <c r="E27" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="F27" s="6" t="s">
+      <c r="F27" s="5" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="28" spans="1:6">
-      <c r="A28" s="5">
-        <v>1</v>
-      </c>
-      <c r="B28" s="6">
-        <v>1</v>
-      </c>
-      <c r="C28" s="6" t="s">
+      <c r="A28" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="B28" s="8"/>
+      <c r="C28" s="8"/>
+      <c r="D28" s="8"/>
+      <c r="E28" s="8"/>
+      <c r="F28" s="8"/>
+    </row>
+    <row r="29" spans="1:6">
+      <c r="A29" s="4">
+        <v>1</v>
+      </c>
+      <c r="B29" s="5">
+        <v>1</v>
+      </c>
+      <c r="C29" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="D28" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="E28" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="F28" s="6" t="s">
+      <c r="D29" s="6" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="29" spans="1:6">
-      <c r="A29" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="B29" s="4"/>
-      <c r="C29" s="4"/>
-      <c r="D29" s="4"/>
-      <c r="E29" s="4"/>
-      <c r="F29" s="4"/>
-    </row>
-    <row r="30" spans="1:6">
-      <c r="A30" s="5">
-        <v>1</v>
-      </c>
-      <c r="B30" s="6">
-        <v>1</v>
-      </c>
-      <c r="C30" s="6" t="s">
+      <c r="E29" s="5" t="s">
         <v>30</v>
       </c>
+      <c r="F29" s="5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" ht="45">
+      <c r="A30" s="4">
+        <v>7</v>
+      </c>
+      <c r="B30" s="5">
+        <v>7</v>
+      </c>
+      <c r="C30" s="5" t="s">
+        <v>32</v>
+      </c>
       <c r="D30" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="E30" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="F30" s="5" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" ht="45">
+      <c r="A31" s="4">
+        <v>7</v>
+      </c>
+      <c r="B31" s="5">
+        <v>7</v>
+      </c>
+      <c r="C31" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="D31" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="E31" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="F31" s="5" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6">
+      <c r="A32" s="4">
+        <v>1</v>
+      </c>
+      <c r="B32" s="5">
+        <v>1</v>
+      </c>
+      <c r="C32" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="D32" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="E32" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="F32" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="E30" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="F30" s="6" t="s">
+    </row>
+    <row r="33" spans="1:6">
+      <c r="A33" s="4">
+        <v>1</v>
+      </c>
+      <c r="B33" s="5">
+        <v>1</v>
+      </c>
+      <c r="C33" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="D33" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="E33" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="F33" s="5" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="31" spans="1:6">
-      <c r="A31" s="5">
-        <v>1</v>
-      </c>
-      <c r="B31" s="6">
-        <v>1</v>
-      </c>
-      <c r="C31" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="D31" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="E31" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="F31" s="6" t="s">
+    <row r="34" spans="1:6">
+      <c r="A34" s="4">
+        <v>1</v>
+      </c>
+      <c r="B34" s="5">
+        <v>1</v>
+      </c>
+      <c r="C34" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="D34" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="E34" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="F34" s="5" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="32" spans="1:6">
-      <c r="A32" s="5">
-        <v>1</v>
-      </c>
-      <c r="B32" s="6">
-        <v>1</v>
-      </c>
-      <c r="C32" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="D32" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="E32" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="F32" s="6" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6">
-      <c r="A33" s="5">
+    <row r="35" spans="1:6">
+      <c r="A35" s="4">
+        <v>1</v>
+      </c>
+      <c r="B35" s="5">
+        <v>1</v>
+      </c>
+      <c r="C35" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="D35" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="E35" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="F35" s="5" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6">
+      <c r="A36" s="4">
+        <v>1</v>
+      </c>
+      <c r="B36" s="5">
+        <v>1</v>
+      </c>
+      <c r="C36" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="D36" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="E36" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="F36" s="5" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6">
+      <c r="A37" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="B37" s="8"/>
+      <c r="C37" s="8"/>
+      <c r="D37" s="8"/>
+      <c r="E37" s="8"/>
+      <c r="F37" s="8"/>
+    </row>
+    <row r="38" spans="1:6">
+      <c r="A38" s="4">
         <v>4</v>
       </c>
-      <c r="B33" s="6">
+      <c r="B38" s="5">
         <v>4</v>
       </c>
-      <c r="C33" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="D33" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="E33" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="F33" s="6" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6">
-      <c r="A34" s="5">
-        <v>1</v>
-      </c>
-      <c r="B34" s="6">
-        <v>1</v>
-      </c>
-      <c r="C34" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="D34" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="E34" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="F34" s="6" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6">
-      <c r="A35" s="5">
-        <v>1</v>
-      </c>
-      <c r="B35" s="6">
-        <v>1</v>
-      </c>
-      <c r="C35" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="D35" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="E35" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="F35" s="6" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6">
-      <c r="A36" s="5">
-        <v>4</v>
-      </c>
-      <c r="B36" s="6">
-        <v>4</v>
-      </c>
-      <c r="C36" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="D36" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="E36" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="F36" s="6" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6">
-      <c r="A37" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B37" s="4"/>
-      <c r="C37" s="4"/>
-      <c r="D37" s="4"/>
-      <c r="E37" s="4"/>
-      <c r="F37" s="4"/>
-    </row>
-    <row r="38" spans="1:6">
-      <c r="A38" s="5">
-        <v>4</v>
-      </c>
-      <c r="B38" s="6">
-        <v>4</v>
-      </c>
-      <c r="C38" s="6" t="s">
+      <c r="C38" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="D38" s="6" t="s">
+      <c r="D38" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="E38" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="F38" s="6" t="s">
+      <c r="E38" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="F38" s="5" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="39" spans="1:6">
-      <c r="A39" s="5">
-        <v>1</v>
-      </c>
-      <c r="B39" s="6">
-        <v>1</v>
-      </c>
-      <c r="C39" s="6" t="s">
+      <c r="A39" s="4">
+        <v>1</v>
+      </c>
+      <c r="B39" s="5">
+        <v>1</v>
+      </c>
+      <c r="C39" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="D39" s="6" t="s">
+      <c r="D39" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="E39" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="F39" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="E39" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="F39" s="6" t="s">
+    </row>
+    <row r="40" spans="1:6">
+      <c r="A40" s="4">
+        <v>1</v>
+      </c>
+      <c r="B40" s="5">
+        <v>1</v>
+      </c>
+      <c r="C40" s="5" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="40" spans="1:6">
-      <c r="A40" s="5">
-        <v>1</v>
-      </c>
-      <c r="B40" s="6">
-        <v>1</v>
-      </c>
-      <c r="C40" s="6" t="s">
+      <c r="D40" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="D40" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="E40" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="F40" s="6" t="s">
+      <c r="E40" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="F40" s="5" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="41" spans="1:6">
-      <c r="A41" s="5">
-        <v>1</v>
-      </c>
-      <c r="B41" s="6">
-        <v>1</v>
-      </c>
-      <c r="C41" s="6" t="s">
+      <c r="A41" s="4">
+        <v>1</v>
+      </c>
+      <c r="B41" s="5">
+        <v>1</v>
+      </c>
+      <c r="C41" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="D41" s="6" t="s">
+      <c r="D41" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="E41" s="6" t="s">
+      <c r="E41" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="F41" s="6" t="s">
+      <c r="F41" s="5" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="42" spans="1:6">
-      <c r="A42" s="4" t="s">
+      <c r="A42" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="B42" s="4"/>
-      <c r="C42" s="4"/>
-      <c r="D42" s="4"/>
-      <c r="E42" s="4"/>
-      <c r="F42" s="4"/>
+      <c r="B42" s="8"/>
+      <c r="C42" s="8"/>
+      <c r="D42" s="8"/>
+      <c r="E42" s="8"/>
+      <c r="F42" s="8"/>
     </row>
     <row r="43" spans="1:6">
-      <c r="A43" s="5">
-        <v>1</v>
-      </c>
-      <c r="B43" s="6">
-        <v>1</v>
-      </c>
-      <c r="C43" s="6" t="s">
+      <c r="A43" s="4">
+        <v>1</v>
+      </c>
+      <c r="B43" s="5">
+        <v>1</v>
+      </c>
+      <c r="C43" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="D43" s="6" t="s">
+      <c r="D43" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="E43" s="6" t="s">
+      <c r="E43" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="F43" s="6" t="s">
+      <c r="F43" s="5" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="44" spans="1:6">
-      <c r="A44" s="4" t="s">
+      <c r="A44" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="B44" s="4"/>
-      <c r="C44" s="4"/>
-      <c r="D44" s="4"/>
-      <c r="E44" s="4"/>
-      <c r="F44" s="4"/>
+      <c r="B44" s="8"/>
+      <c r="C44" s="8"/>
+      <c r="D44" s="8"/>
+      <c r="E44" s="8"/>
+      <c r="F44" s="8"/>
     </row>
     <row r="45" spans="1:6">
-      <c r="A45" s="5">
-        <v>1</v>
-      </c>
-      <c r="B45" s="6">
-        <v>1</v>
-      </c>
-      <c r="C45" s="6" t="s">
+      <c r="A45" s="4">
+        <v>1</v>
+      </c>
+      <c r="B45" s="5">
+        <v>1</v>
+      </c>
+      <c r="C45" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="D45" s="6" t="s">
+      <c r="D45" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="E45" s="6" t="s">
+      <c r="E45" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="F45" s="6" t="s">
+      <c r="F45" s="5" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="46" spans="1:6">
-      <c r="A46" s="5">
-        <v>1</v>
-      </c>
-      <c r="B46" s="6">
-        <v>1</v>
-      </c>
-      <c r="C46" s="6" t="s">
+      <c r="A46" s="4">
+        <v>1</v>
+      </c>
+      <c r="B46" s="5">
+        <v>1</v>
+      </c>
+      <c r="C46" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="D46" s="6" t="s">
+      <c r="D46" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="E46" s="6" t="s">
+      <c r="E46" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="F46" s="6" t="s">
+      <c r="F46" s="5" t="s">
         <v>69</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="A44:F44"/>
+    <mergeCell ref="A11:F11"/>
+    <mergeCell ref="A25:F25"/>
+    <mergeCell ref="A28:F28"/>
+    <mergeCell ref="A37:F37"/>
+    <mergeCell ref="A42:F42"/>
+    <mergeCell ref="A6:F6"/>
+    <mergeCell ref="A7:F7"/>
+    <mergeCell ref="A8:F8"/>
+    <mergeCell ref="A9:F9"/>
+    <mergeCell ref="A10:F10"/>
     <mergeCell ref="A1:F1"/>
     <mergeCell ref="A2:F2"/>
     <mergeCell ref="A3:F3"/>
     <mergeCell ref="A4:F4"/>
     <mergeCell ref="A5:F5"/>
-    <mergeCell ref="A6:F6"/>
-    <mergeCell ref="A7:F7"/>
-    <mergeCell ref="A8:F8"/>
-    <mergeCell ref="A9:F9"/>
-    <mergeCell ref="A10:F10"/>
-    <mergeCell ref="A11:F11"/>
-    <mergeCell ref="A25:F25"/>
-    <mergeCell ref="A29:F29"/>
-    <mergeCell ref="A37:F37"/>
-    <mergeCell ref="A42:F42"/>
-    <mergeCell ref="A44:F44"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
shield 4.3: fix display connectors position. Regenerate output file. Release pcb ver.E
</commit_message>
<xml_diff>
--- a/Assembly/shield_display_4.3/bom-shield_display_4.3.xlsx
+++ b/Assembly/shield_display_4.3/bom-shield_display_4.3.xlsx
@@ -14,21 +14,39 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="98">
   <si>
     <t>Bill of Materials</t>
   </si>
   <si>
-    <t>Date: 23/11/2019</t>
-  </si>
-  <si>
-    <t>Project: Shield 4.3'' Display LCD PCAP PN: -</t>
-  </si>
-  <si>
-    <t>Hardware_version: 2</t>
-  </si>
-  <si>
-    <t>PCB_version: C</t>
+    <t>Generation Date: 12/02/2020</t>
+  </si>
+  <si>
+    <t>Project Date: 19/01/2016</t>
+  </si>
+  <si>
+    <t>Hardware Version: 2</t>
+  </si>
+  <si>
+    <t>PCB Version: D</t>
+  </si>
+  <si>
+    <t>Project Name: Shield 4.3'' Display</t>
+  </si>
+  <si>
+    <t>License: MIT</t>
+  </si>
+  <si>
+    <t>Descriptions: Shield 4.3'' Display LCD PCAP</t>
+  </si>
+  <si>
+    <t>Part Number: -</t>
+  </si>
+  <si>
+    <t>Project status: Reference</t>
+  </si>
+  <si>
+    <t>Project group: -</t>
   </si>
   <si>
     <t>BOM files:</t>
@@ -40,6 +58,33 @@
     <t>Statistics</t>
   </si>
   <si>
+    <t>Merged Files Number</t>
+  </si>
+  <si>
+    <t>Components:</t>
+  </si>
+  <si>
+    <t>Connectors and holders</t>
+  </si>
+  <si>
+    <t>Mechanical parts and buttons</t>
+  </si>
+  <si>
+    <t>Resistor components</t>
+  </si>
+  <si>
+    <t>Capacitors</t>
+  </si>
+  <si>
+    <t>L  Inductors, chokes</t>
+  </si>
+  <si>
+    <t>Integrates and chips</t>
+  </si>
+  <si>
+    <t>Total BOM Componets</t>
+  </si>
+  <si>
     <t>NP=NOT POPULATE (NON MONTARE)!</t>
   </si>
   <si>
@@ -64,34 +109,34 @@
     <t>J * Connectors and holders *</t>
   </si>
   <si>
-    <t>J5</t>
+    <t>J1, J2, J3</t>
   </si>
   <si>
     <t>Connector</t>
   </si>
   <si>
+    <t>SOCKET_2x26_2.54MM_THD</t>
+  </si>
+  <si>
+    <t>Socket Header, 52 pin, 26x2, 2.54mm, H=8.5mm</t>
+  </si>
+  <si>
+    <t>J4</t>
+  </si>
+  <si>
+    <t>FCC-ZIF_40PIN_0.5MM_TOP_LOWPROFILE</t>
+  </si>
+  <si>
+    <t>Connectors, FPC, SMT ZIF, Low Profile, Horizontal, Top Contact, pitch 0.5 mm, 40 pins (WE 687140183622)</t>
+  </si>
+  <si>
+    <t>J5, J6</t>
+  </si>
+  <si>
     <t>FCC-ZIF_10PIN_0.5MM_LOW_PROFILE</t>
   </si>
   <si>
-    <t>Connectors, FPC, SMT ZIF, Low Profile, Horizontal, Top Contact, pitch 0.5 mm, 10 pins (WE 687110183622)</t>
-  </si>
-  <si>
-    <t>J1, J2, J3</t>
-  </si>
-  <si>
-    <t>SOCKET_2x26_2.54MM_THD</t>
-  </si>
-  <si>
-    <t>Socket Header, 52 pin, 26x2, 2.54mm, H=8.5mm</t>
-  </si>
-  <si>
-    <t>J4</t>
-  </si>
-  <si>
-    <t>FCC-ZIF_40PIN_0.5MM_TOP_LOWPROFILE</t>
-  </si>
-  <si>
-    <t>Connectors, FPC, SMT ZIF, Low Profile, Horizontal, Top Contact, pitch 0.5 mm, 40 pins (WE 687140183622)</t>
+    <t>Connectors, FPC, SMT ZIF, Low Profile, Horizontal, Top Contact, pitch 0.5 mm, 10 pins (WE 687110183622), Connectors, FPC, SMT ZIF, Low Profile, Horizontal, BOT Contact, pitch 0.5 mm, 10 pins (WE )</t>
   </si>
   <si>
     <t>S * Mechanical parts and buttons *</t>
@@ -193,7 +238,7 @@
     <t>C * Capacitors *</t>
   </si>
   <si>
-    <t>C1, C2, C3, C6, C7, C8, C9, C10, C11, C12</t>
+    <t>C1, C2, C3, C6, C7, C8, C9, C10, C11, C12, C13</t>
   </si>
   <si>
     <t>100nF</t>
@@ -269,7 +314,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -279,6 +324,14 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -310,7 +363,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -320,6 +373,24 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF00CCCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC0C0C0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF66B2FF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF4C9900"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -369,7 +440,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -377,20 +448,35 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -687,16 +773,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F46"/>
+  <dimension ref="A1:F61"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="3" max="46" width="50.7109375" customWidth="1"/>
-    <col min="4" max="46" width="50.7109375" customWidth="1"/>
-    <col min="5" max="46" width="50.7109375" customWidth="1"/>
-    <col min="6" max="46" width="50.7109375" customWidth="1"/>
+    <col min="3" max="61" width="50.7109375" customWidth="1"/>
+    <col min="4" max="61" width="50.7109375" customWidth="1"/>
+    <col min="5" max="61" width="50.7109375" customWidth="1"/>
+    <col min="6" max="61" width="50.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -774,7 +860,9 @@
       <c r="F8" s="1"/>
     </row>
     <row r="9" spans="1:6">
-      <c r="A9" s="1"/>
+      <c r="A9" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
@@ -783,7 +871,7 @@
     </row>
     <row r="10" spans="1:6">
       <c r="A10" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
@@ -793,7 +881,7 @@
     </row>
     <row r="11" spans="1:6">
       <c r="A11" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
@@ -801,37 +889,71 @@
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
     </row>
+    <row r="12" spans="1:6">
+      <c r="A12" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B12" s="1"/>
+      <c r="C12" s="1"/>
+      <c r="D12" s="1"/>
+      <c r="E12" s="1"/>
+      <c r="F12" s="1"/>
+    </row>
     <row r="13" spans="1:6">
-      <c r="A13" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B13" s="2"/>
-      <c r="C13" s="2"/>
+      <c r="A13" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B13" s="1"/>
+      <c r="C13" s="1"/>
+      <c r="D13" s="1"/>
+      <c r="E13" s="1"/>
+      <c r="F13" s="1"/>
+    </row>
+    <row r="14" spans="1:6">
+      <c r="A14" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B14" s="1"/>
+      <c r="C14" s="1"/>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1"/>
+      <c r="F14" s="1"/>
     </row>
     <row r="15" spans="1:6">
-      <c r="A15" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6">
-      <c r="A17" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B17" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C17" s="4" t="s">
+      <c r="A15" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="D17" s="4" t="s">
+      <c r="B15" s="1"/>
+      <c r="C15" s="1"/>
+      <c r="D15" s="1"/>
+      <c r="E15" s="1"/>
+      <c r="F15" s="1"/>
+    </row>
+    <row r="16" spans="1:6">
+      <c r="A16" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="E17" s="4" t="s">
+      <c r="B16" s="1"/>
+      <c r="C16" s="1"/>
+      <c r="D16" s="1"/>
+      <c r="E16" s="1"/>
+      <c r="F16" s="1"/>
+    </row>
+    <row r="18" spans="1:6">
+      <c r="A18" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="F17" s="4" t="s">
+      <c r="B18" s="2"/>
+      <c r="C18" s="2"/>
+    </row>
+    <row r="19" spans="1:6">
+      <c r="A19" s="3">
+        <v>1</v>
+      </c>
+      <c r="B19" s="4" t="s">
         <v>14</v>
       </c>
+      <c r="C19" s="4"/>
     </row>
     <row r="20" spans="1:6">
       <c r="A20" s="5" t="s">
@@ -839,482 +961,577 @@
       </c>
       <c r="B20" s="5"/>
       <c r="C20" s="5"/>
-      <c r="D20" s="5"/>
-      <c r="E20" s="5"/>
-      <c r="F20" s="5"/>
     </row>
     <row r="21" spans="1:6">
-      <c r="A21" s="6">
-        <v>1</v>
-      </c>
-      <c r="B21" s="7">
-        <v>1</v>
-      </c>
-      <c r="C21" s="7" t="s">
+      <c r="A21" s="3">
+        <v>6</v>
+      </c>
+      <c r="B21" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="D21" s="7" t="s">
+      <c r="C21" s="4"/>
+    </row>
+    <row r="22" spans="1:6">
+      <c r="A22" s="3">
+        <v>4</v>
+      </c>
+      <c r="B22" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="E21" s="7" t="s">
+      <c r="C22" s="4"/>
+    </row>
+    <row r="23" spans="1:6">
+      <c r="A23" s="3">
+        <v>24</v>
+      </c>
+      <c r="B23" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="F21" s="7" t="s">
+      <c r="C23" s="4"/>
+    </row>
+    <row r="24" spans="1:6">
+      <c r="A24" s="3">
+        <v>13</v>
+      </c>
+      <c r="B24" s="4" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="22" spans="1:6">
-      <c r="A22" s="6">
-        <v>3</v>
-      </c>
-      <c r="B22" s="7">
-        <v>3</v>
-      </c>
-      <c r="C22" s="7" t="s">
+      <c r="C24" s="4"/>
+    </row>
+    <row r="25" spans="1:6">
+      <c r="A25" s="3">
+        <v>1</v>
+      </c>
+      <c r="B25" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="D22" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="E22" s="7" t="s">
+      <c r="C25" s="4"/>
+    </row>
+    <row r="26" spans="1:6">
+      <c r="A26" s="3">
+        <v>2</v>
+      </c>
+      <c r="B26" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="F22" s="7" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6">
-      <c r="A23" s="6">
-        <v>1</v>
-      </c>
-      <c r="B23" s="7">
-        <v>1</v>
-      </c>
-      <c r="C23" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="D23" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="E23" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="F23" s="7" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6">
-      <c r="A24" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="B24" s="5"/>
-      <c r="C24" s="5"/>
-      <c r="D24" s="5"/>
-      <c r="E24" s="5"/>
-      <c r="F24" s="5"/>
-    </row>
-    <row r="25" spans="1:6">
-      <c r="A25" s="6">
-        <v>4</v>
-      </c>
-      <c r="B25" s="7">
-        <v>4</v>
-      </c>
-      <c r="C25" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="D25" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="E25" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="F25" s="7" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6">
-      <c r="A26" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="B26" s="5"/>
-      <c r="C26" s="5"/>
-      <c r="D26" s="5"/>
-      <c r="E26" s="5"/>
-      <c r="F26" s="5"/>
+      <c r="C26" s="4"/>
     </row>
     <row r="27" spans="1:6">
       <c r="A27" s="6">
+        <v>50</v>
+      </c>
+      <c r="B27" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="C27" s="7"/>
+    </row>
+    <row r="30" spans="1:6">
+      <c r="A30" s="8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6">
+      <c r="A32" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="B32" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="C32" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="D32" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="E32" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="F32" s="9" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6">
+      <c r="A35" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="B35" s="10"/>
+      <c r="C35" s="10"/>
+      <c r="D35" s="10"/>
+      <c r="E35" s="10"/>
+      <c r="F35" s="10"/>
+    </row>
+    <row r="36" spans="1:6">
+      <c r="A36" s="11">
+        <v>3</v>
+      </c>
+      <c r="B36" s="12">
+        <v>3</v>
+      </c>
+      <c r="C36" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="D36" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="E36" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="F36" s="12" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6">
+      <c r="A37" s="11">
+        <v>1</v>
+      </c>
+      <c r="B37" s="12">
+        <v>1</v>
+      </c>
+      <c r="C37" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="D37" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="E37" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="F37" s="12" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6">
+      <c r="A38" s="11">
+        <v>2</v>
+      </c>
+      <c r="B38" s="12">
+        <v>2</v>
+      </c>
+      <c r="C38" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="D38" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="E38" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="F38" s="12" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6">
+      <c r="A39" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="B39" s="10"/>
+      <c r="C39" s="10"/>
+      <c r="D39" s="10"/>
+      <c r="E39" s="10"/>
+      <c r="F39" s="10"/>
+    </row>
+    <row r="40" spans="1:6">
+      <c r="A40" s="11">
+        <v>4</v>
+      </c>
+      <c r="B40" s="12">
+        <v>4</v>
+      </c>
+      <c r="C40" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="D40" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="E40" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="F40" s="12" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6">
+      <c r="A41" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="B41" s="10"/>
+      <c r="C41" s="10"/>
+      <c r="D41" s="10"/>
+      <c r="E41" s="10"/>
+      <c r="F41" s="10"/>
+    </row>
+    <row r="42" spans="1:6">
+      <c r="A42" s="11">
         <v>5</v>
       </c>
-      <c r="B27" s="7">
+      <c r="B42" s="12">
         <v>5</v>
       </c>
-      <c r="C27" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="D27" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="E27" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="F27" s="7" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6">
-      <c r="A28" s="6">
+      <c r="C42" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="D42" s="13" t="s">
+        <v>48</v>
+      </c>
+      <c r="E42" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="F42" s="12" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6">
+      <c r="A43" s="11">
         <v>3</v>
       </c>
-      <c r="B28" s="7">
+      <c r="B43" s="12">
         <v>3</v>
       </c>
-      <c r="C28" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="D28" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="E28" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="F28" s="7" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6">
-      <c r="A29" s="6">
-        <v>1</v>
-      </c>
-      <c r="B29" s="7">
-        <v>1</v>
-      </c>
-      <c r="C29" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="D29" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="E29" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="F29" s="7" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6">
-      <c r="A30" s="6">
+      <c r="C43" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="D43" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="E43" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="F43" s="12" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6">
+      <c r="A44" s="11">
+        <v>1</v>
+      </c>
+      <c r="B44" s="12">
+        <v>1</v>
+      </c>
+      <c r="C44" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="D44" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="E44" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="F44" s="12" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6">
+      <c r="A45" s="11">
         <v>4</v>
       </c>
-      <c r="B30" s="7">
+      <c r="B45" s="12">
         <v>4</v>
       </c>
-      <c r="C30" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="D30" s="7" t="s">
-        <v>43</v>
-      </c>
-      <c r="E30" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="F30" s="7" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6">
-      <c r="A31" s="6">
+      <c r="C45" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="D45" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="E45" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="F45" s="12" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6">
+      <c r="A46" s="11">
         <v>4</v>
       </c>
-      <c r="B31" s="7">
+      <c r="B46" s="12">
         <v>4</v>
       </c>
-      <c r="C31" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="D31" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="E31" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="F31" s="7" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6">
-      <c r="A32" s="6">
-        <v>1</v>
-      </c>
-      <c r="B32" s="7">
-        <v>1</v>
-      </c>
-      <c r="C32" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="D32" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="E32" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="F32" s="7" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6">
-      <c r="A33" s="6">
+      <c r="C46" s="12" t="s">
+        <v>59</v>
+      </c>
+      <c r="D46" s="12" t="s">
+        <v>60</v>
+      </c>
+      <c r="E46" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="F46" s="12" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6">
+      <c r="A47" s="11">
+        <v>1</v>
+      </c>
+      <c r="B47" s="12">
+        <v>1</v>
+      </c>
+      <c r="C47" s="12" t="s">
+        <v>61</v>
+      </c>
+      <c r="D47" s="12" t="s">
+        <v>62</v>
+      </c>
+      <c r="E47" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="F47" s="12" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6">
+      <c r="A48" s="11">
         <v>2</v>
       </c>
-      <c r="B33" s="7">
+      <c r="B48" s="12">
         <v>2</v>
       </c>
-      <c r="C33" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="D33" s="7" t="s">
+      <c r="C48" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="D48" s="12" t="s">
+        <v>64</v>
+      </c>
+      <c r="E48" s="12" t="s">
         <v>49</v>
       </c>
-      <c r="E33" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="F33" s="7" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6">
-      <c r="A34" s="6">
-        <v>1</v>
-      </c>
-      <c r="B34" s="7">
-        <v>1</v>
-      </c>
-      <c r="C34" s="7" t="s">
-        <v>50</v>
-      </c>
-      <c r="D34" s="7" t="s">
-        <v>51</v>
-      </c>
-      <c r="E34" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="F34" s="7" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6">
-      <c r="A35" s="6">
-        <v>1</v>
-      </c>
-      <c r="B35" s="7">
-        <v>1</v>
-      </c>
-      <c r="C35" s="7" t="s">
-        <v>52</v>
-      </c>
-      <c r="D35" s="7" t="s">
+      <c r="F48" s="12" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6">
+      <c r="A49" s="11">
+        <v>1</v>
+      </c>
+      <c r="B49" s="12">
+        <v>1</v>
+      </c>
+      <c r="C49" s="12" t="s">
+        <v>65</v>
+      </c>
+      <c r="D49" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="E49" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="F49" s="12" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6">
+      <c r="A50" s="11">
+        <v>1</v>
+      </c>
+      <c r="B50" s="12">
+        <v>1</v>
+      </c>
+      <c r="C50" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="D50" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="E50" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="F50" s="12" t="s">
         <v>53</v>
       </c>
-      <c r="E35" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="F35" s="7" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6">
-      <c r="A36" s="6">
-        <v>1</v>
-      </c>
-      <c r="B36" s="7">
-        <v>1</v>
-      </c>
-      <c r="C36" s="7" t="s">
-        <v>54</v>
-      </c>
-      <c r="D36" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="E36" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="F36" s="7" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6">
-      <c r="A37" s="6">
-        <v>1</v>
-      </c>
-      <c r="B37" s="7">
-        <v>1</v>
-      </c>
-      <c r="C37" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="D37" s="7" t="s">
-        <v>57</v>
-      </c>
-      <c r="E37" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="F37" s="7" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6">
-      <c r="A38" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="B38" s="5"/>
-      <c r="C38" s="5"/>
-      <c r="D38" s="5"/>
-      <c r="E38" s="5"/>
-      <c r="F38" s="5"/>
-    </row>
-    <row r="39" spans="1:6">
-      <c r="A39" s="6">
-        <v>10</v>
-      </c>
-      <c r="B39" s="7">
-        <v>10</v>
-      </c>
-      <c r="C39" s="7" t="s">
-        <v>59</v>
-      </c>
-      <c r="D39" s="7" t="s">
-        <v>60</v>
-      </c>
-      <c r="E39" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="F39" s="7" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6">
-      <c r="A40" s="6">
-        <v>1</v>
-      </c>
-      <c r="B40" s="7">
-        <v>1</v>
-      </c>
-      <c r="C40" s="7" t="s">
-        <v>62</v>
-      </c>
-      <c r="D40" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="E40" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="F40" s="7" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6">
-      <c r="A41" s="6">
-        <v>1</v>
-      </c>
-      <c r="B41" s="7">
-        <v>1</v>
-      </c>
-      <c r="C41" s="7" t="s">
-        <v>65</v>
-      </c>
-      <c r="D41" s="7" t="s">
-        <v>66</v>
-      </c>
-      <c r="E41" s="7" t="s">
-        <v>67</v>
-      </c>
-      <c r="F41" s="7" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6">
-      <c r="A42" s="5" t="s">
+    </row>
+    <row r="51" spans="1:6">
+      <c r="A51" s="11">
+        <v>1</v>
+      </c>
+      <c r="B51" s="12">
+        <v>1</v>
+      </c>
+      <c r="C51" s="12" t="s">
         <v>69</v>
       </c>
-      <c r="B42" s="5"/>
-      <c r="C42" s="5"/>
-      <c r="D42" s="5"/>
-      <c r="E42" s="5"/>
-      <c r="F42" s="5"/>
-    </row>
-    <row r="43" spans="1:6">
-      <c r="A43" s="6">
-        <v>1</v>
-      </c>
-      <c r="B43" s="7">
-        <v>1</v>
-      </c>
-      <c r="C43" s="7" t="s">
+      <c r="D51" s="12" t="s">
         <v>70</v>
       </c>
-      <c r="D43" s="7" t="s">
+      <c r="E51" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="F51" s="12" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6">
+      <c r="A52" s="11">
+        <v>1</v>
+      </c>
+      <c r="B52" s="12">
+        <v>1</v>
+      </c>
+      <c r="C52" s="12" t="s">
         <v>71</v>
       </c>
-      <c r="E43" s="7" t="s">
+      <c r="D52" s="12" t="s">
         <v>72</v>
       </c>
-      <c r="F43" s="7" t="s">
+      <c r="E52" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="F52" s="12" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6">
+      <c r="A53" s="10" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="44" spans="1:6">
-      <c r="A44" s="5" t="s">
+      <c r="B53" s="10"/>
+      <c r="C53" s="10"/>
+      <c r="D53" s="10"/>
+      <c r="E53" s="10"/>
+      <c r="F53" s="10"/>
+    </row>
+    <row r="54" spans="1:6">
+      <c r="A54" s="11">
+        <v>11</v>
+      </c>
+      <c r="B54" s="12">
+        <v>11</v>
+      </c>
+      <c r="C54" s="12" t="s">
         <v>74</v>
       </c>
-      <c r="B44" s="5"/>
-      <c r="C44" s="5"/>
-      <c r="D44" s="5"/>
-      <c r="E44" s="5"/>
-      <c r="F44" s="5"/>
-    </row>
-    <row r="45" spans="1:6">
-      <c r="A45" s="6">
-        <v>1</v>
-      </c>
-      <c r="B45" s="7">
-        <v>1</v>
-      </c>
-      <c r="C45" s="7" t="s">
+      <c r="D54" s="12" t="s">
         <v>75</v>
       </c>
-      <c r="D45" s="7" t="s">
+      <c r="E54" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="F54" s="12" t="s">
         <v>76</v>
       </c>
-      <c r="E45" s="7" t="s">
+    </row>
+    <row r="55" spans="1:6">
+      <c r="A55" s="11">
+        <v>1</v>
+      </c>
+      <c r="B55" s="12">
+        <v>1</v>
+      </c>
+      <c r="C55" s="12" t="s">
         <v>77</v>
       </c>
-      <c r="F45" s="7" t="s">
+      <c r="D55" s="12" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="46" spans="1:6">
-      <c r="A46" s="6">
-        <v>1</v>
-      </c>
-      <c r="B46" s="7">
-        <v>1</v>
-      </c>
-      <c r="C46" s="7" t="s">
+      <c r="E55" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="F55" s="12" t="s">
         <v>79</v>
       </c>
-      <c r="D46" s="7" t="s">
+    </row>
+    <row r="56" spans="1:6">
+      <c r="A56" s="11">
+        <v>1</v>
+      </c>
+      <c r="B56" s="12">
+        <v>1</v>
+      </c>
+      <c r="C56" s="12" t="s">
         <v>80</v>
       </c>
-      <c r="E46" s="7" t="s">
+      <c r="D56" s="12" t="s">
         <v>81</v>
       </c>
-      <c r="F46" s="7" t="s">
+      <c r="E56" s="12" t="s">
         <v>82</v>
       </c>
+      <c r="F56" s="12" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6">
+      <c r="A57" s="10" t="s">
+        <v>84</v>
+      </c>
+      <c r="B57" s="10"/>
+      <c r="C57" s="10"/>
+      <c r="D57" s="10"/>
+      <c r="E57" s="10"/>
+      <c r="F57" s="10"/>
+    </row>
+    <row r="58" spans="1:6">
+      <c r="A58" s="11">
+        <v>1</v>
+      </c>
+      <c r="B58" s="12">
+        <v>1</v>
+      </c>
+      <c r="C58" s="12" t="s">
+        <v>85</v>
+      </c>
+      <c r="D58" s="12" t="s">
+        <v>86</v>
+      </c>
+      <c r="E58" s="12" t="s">
+        <v>87</v>
+      </c>
+      <c r="F58" s="12" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6">
+      <c r="A59" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="B59" s="10"/>
+      <c r="C59" s="10"/>
+      <c r="D59" s="10"/>
+      <c r="E59" s="10"/>
+      <c r="F59" s="10"/>
+    </row>
+    <row r="60" spans="1:6">
+      <c r="A60" s="11">
+        <v>1</v>
+      </c>
+      <c r="B60" s="12">
+        <v>1</v>
+      </c>
+      <c r="C60" s="12" t="s">
+        <v>90</v>
+      </c>
+      <c r="D60" s="12" t="s">
+        <v>91</v>
+      </c>
+      <c r="E60" s="12" t="s">
+        <v>92</v>
+      </c>
+      <c r="F60" s="12" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6">
+      <c r="A61" s="11">
+        <v>1</v>
+      </c>
+      <c r="B61" s="12">
+        <v>1</v>
+      </c>
+      <c r="C61" s="12" t="s">
+        <v>94</v>
+      </c>
+      <c r="D61" s="12" t="s">
+        <v>95</v>
+      </c>
+      <c r="E61" s="12" t="s">
+        <v>96</v>
+      </c>
+      <c r="F61" s="12" t="s">
+        <v>97</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="18">
+  <mergeCells count="32">
     <mergeCell ref="A1:F1"/>
     <mergeCell ref="A2:F2"/>
     <mergeCell ref="A3:F3"/>
@@ -1326,13 +1543,27 @@
     <mergeCell ref="A9:F9"/>
     <mergeCell ref="A10:F10"/>
     <mergeCell ref="A11:F11"/>
-    <mergeCell ref="A13:C13"/>
-    <mergeCell ref="A20:F20"/>
-    <mergeCell ref="A24:F24"/>
-    <mergeCell ref="A26:F26"/>
-    <mergeCell ref="A38:F38"/>
-    <mergeCell ref="A42:F42"/>
-    <mergeCell ref="A44:F44"/>
+    <mergeCell ref="A12:F12"/>
+    <mergeCell ref="A13:F13"/>
+    <mergeCell ref="A14:F14"/>
+    <mergeCell ref="A15:F15"/>
+    <mergeCell ref="A16:F16"/>
+    <mergeCell ref="A18:C18"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="A20:C20"/>
+    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="B22:C22"/>
+    <mergeCell ref="B23:C23"/>
+    <mergeCell ref="B24:C24"/>
+    <mergeCell ref="B25:C25"/>
+    <mergeCell ref="B26:C26"/>
+    <mergeCell ref="B27:C27"/>
+    <mergeCell ref="A35:F35"/>
+    <mergeCell ref="A39:F39"/>
+    <mergeCell ref="A41:F41"/>
+    <mergeCell ref="A53:F53"/>
+    <mergeCell ref="A57:F57"/>
+    <mergeCell ref="A59:F59"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>